<commit_message>
Apparently I had never actually gone back and fixed edited3 and edited4 (and therefore edited6) to delete the non-Sonoran species for location-independent, butI did that now
</commit_message>
<xml_diff>
--- a/Sonoran-data/data-wrangling-intermediate/01b_edited7_location-dependent-manual-fix.xlsx
+++ b/Sonoran-data/data-wrangling-intermediate/01b_edited7_location-dependent-manual-fix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eltnmsu-my.sharepoint.com/personal/lossanna_nmsu_edu/Documents/Documents/02_RestoreNet/RestoreNet/Sonoran-data/data-wrangling-intermediate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="8_{C3EF6CDF-594F-4BE4-9EF4-7E0609E88FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4D46A40-EAC4-4DC1-9F0B-0C3D91A728FF}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="8_{C3EF6CDF-594F-4BE4-9EF4-7E0609E88FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F5255B1-CBE8-474F-BB97-2E6F7B2EEFDB}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{A09795D3-E60D-44CB-9C72-087875526995}"/>
+    <workbookView minimized="1" xWindow="3708" yWindow="3588" windowWidth="17280" windowHeight="9156" xr2:uid="{A09795D3-E60D-44CB-9C72-087875526995}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1297,7 +1297,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E65" sqref="E65"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
So in theory I have corrected both species lists for the subplot data
</commit_message>
<xml_diff>
--- a/Sonoran-data/data-wrangling-intermediate/01b_edited7_location-dependent-manual-fix.xlsx
+++ b/Sonoran-data/data-wrangling-intermediate/01b_edited7_location-dependent-manual-fix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eltnmsu-my.sharepoint.com/personal/lossanna_nmsu_edu/Documents/Documents/02_RestoreNet/RestoreNet/Sonoran-data/data-wrangling-intermediate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="8_{C3EF6CDF-594F-4BE4-9EF4-7E0609E88FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F5255B1-CBE8-474F-BB97-2E6F7B2EEFDB}"/>
+  <xr:revisionPtr revIDLastSave="92" documentId="8_{C3EF6CDF-594F-4BE4-9EF4-7E0609E88FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1DF47B9E-8CD2-4653-8FF1-C07A2D38710F}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="3708" yWindow="3588" windowWidth="17280" windowHeight="9156" xr2:uid="{A09795D3-E60D-44CB-9C72-087875526995}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{A09795D3-E60D-44CB-9C72-087875526995}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="265">
   <si>
     <t>Region</t>
   </si>
@@ -131,9 +131,6 @@
     <t>BOUSPP</t>
   </si>
   <si>
-    <t>Bouteloua spp., SRER</t>
-  </si>
-  <si>
     <t>BRASPP.SRER</t>
   </si>
   <si>
@@ -581,21 +578,6 @@
     <t>Unknown forb seedling, Patagonia</t>
   </si>
   <si>
-    <t>UNGR1.Patagonia</t>
-  </si>
-  <si>
-    <t>UNGR1</t>
-  </si>
-  <si>
-    <t>Unknown grass 1, Patagonia</t>
-  </si>
-  <si>
-    <t>UNGR1.SRER</t>
-  </si>
-  <si>
-    <t>Unknown grass (SantaRita); Possibly BOER or Aristida spp (so likely unseeded), SRER</t>
-  </si>
-  <si>
     <t>UNGRS1.Patagonia</t>
   </si>
   <si>
@@ -749,15 +731,9 @@
     <t>Cryptantha spp. 2, SRER</t>
   </si>
   <si>
-    <t>CRYSPP2.SRER</t>
-  </si>
-  <si>
     <t>CRYSPP2</t>
   </si>
   <si>
-    <t>Cryptantha spp. 3, SRER</t>
-  </si>
-  <si>
     <t>FESSPP.SRER</t>
   </si>
   <si>
@@ -822,6 +798,39 @@
   </si>
   <si>
     <t>Unknown forb (Patagonia); Umbilliferae family, thin lacey divided leaves with small white flowers in umbels at the top, Patagonia</t>
+  </si>
+  <si>
+    <t>CHSPP.Pleasant</t>
+  </si>
+  <si>
+    <t>CHSPP</t>
+  </si>
+  <si>
+    <t>Chamaesyce spp., Pleasant</t>
+  </si>
+  <si>
+    <t>UNGR1 (possible ERLE).Patagonia</t>
+  </si>
+  <si>
+    <t>UNGR1 (possible ERLE)</t>
+  </si>
+  <si>
+    <t>Unknown grass 1, possibly ERLE, Patagonia</t>
+  </si>
+  <si>
+    <t>UNGR1 (BOER/Aristida).SRER</t>
+  </si>
+  <si>
+    <t>UNGR1 (BOER/Aristida)</t>
+  </si>
+  <si>
+    <t>Unknown grass 1, BOER4 or Aristida, SRER</t>
+  </si>
+  <si>
+    <t>Annual</t>
+  </si>
+  <si>
+    <t>Bouteloua spp. (BOCH, BOCU, BORE, or BORA), SRER</t>
   </si>
 </sst>
 </file>
@@ -863,9 +872,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -888,15 +898,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>388620</xdr:colOff>
+      <xdr:colOff>205740</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>81915</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>441960</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -911,8 +921,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5265420" y="205740"/>
-          <a:ext cx="3284220" cy="1339215"/>
+          <a:off x="10988040" y="297180"/>
+          <a:ext cx="3284220" cy="2385060"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -962,6 +972,15 @@
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
             <a:t>Changed cells are highlighted. Changed native status based on details in name. Switched names between Patagonia &amp; SRER when specified in name.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Code changed for what was formally "CRYSPP2.SRER", because I'm pretty sure it's the same as CRYSPP 2 (with a space).</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
@@ -1293,11 +1312,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6595BD7-2435-430D-9E63-650FB0A0F724}">
-  <dimension ref="A1:H85"/>
+  <dimension ref="A1:H86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11:XFD11"/>
+      <selection pane="bottomLeft" activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1337,22 +1356,22 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>254</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>255</v>
       </c>
       <c r="E2" t="s">
-        <v>48</v>
+        <v>256</v>
       </c>
       <c r="F2" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="G2" t="s">
         <v>14</v>
@@ -1363,19 +1382,19 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" t="s">
         <v>46</v>
       </c>
-      <c r="C3" t="s">
-        <v>59</v>
-      </c>
       <c r="D3" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="E3" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="F3" t="s">
         <v>5</v>
@@ -1389,45 +1408,45 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
-        <v>215</v>
+        <v>58</v>
       </c>
       <c r="D4" t="s">
-        <v>216</v>
+        <v>59</v>
       </c>
       <c r="E4" t="s">
-        <v>217</v>
+        <v>60</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="G4" t="s">
         <v>14</v>
       </c>
       <c r="H4" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C5" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
       <c r="D5" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="E5" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
       <c r="F5" t="s">
         <v>14</v>
@@ -1436,25 +1455,25 @@
         <v>14</v>
       </c>
       <c r="H5" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" t="s">
+        <v>220</v>
+      </c>
+      <c r="D6" t="s">
+        <v>221</v>
+      </c>
+      <c r="E6" t="s">
         <v>222</v>
       </c>
-      <c r="C6" t="s">
-        <v>223</v>
-      </c>
-      <c r="D6" t="s">
-        <v>224</v>
-      </c>
-      <c r="E6" t="s">
-        <v>225</v>
-      </c>
       <c r="F6" t="s">
         <v>14</v>
       </c>
@@ -1462,24 +1481,24 @@
         <v>14</v>
       </c>
       <c r="H6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C7" t="s">
-        <v>255</v>
+        <v>217</v>
       </c>
       <c r="D7" t="s">
-        <v>256</v>
+        <v>218</v>
       </c>
       <c r="E7" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="F7" t="s">
         <v>14</v>
@@ -1493,22 +1512,22 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>216</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>247</v>
       </c>
       <c r="D8" t="s">
-        <v>44</v>
+        <v>248</v>
       </c>
       <c r="E8" t="s">
-        <v>45</v>
+        <v>219</v>
       </c>
       <c r="F8" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="G8" t="s">
         <v>14</v>
@@ -1519,45 +1538,45 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" t="s">
         <v>41</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>42</v>
       </c>
-      <c r="C9" t="s">
-        <v>257</v>
-      </c>
       <c r="D9" t="s">
-        <v>258</v>
+        <v>43</v>
       </c>
       <c r="E9" t="s">
-        <v>259</v>
+        <v>44</v>
       </c>
       <c r="F9" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="G9" t="s">
         <v>14</v>
       </c>
       <c r="H9" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" t="s">
         <v>41</v>
       </c>
-      <c r="B10" t="s">
-        <v>218</v>
-      </c>
       <c r="C10" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D10" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="E10" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F10" t="s">
         <v>14</v>
@@ -1566,85 +1585,85 @@
         <v>14</v>
       </c>
       <c r="H10" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C11" t="s">
-        <v>219</v>
+        <v>244</v>
       </c>
       <c r="D11" t="s">
-        <v>220</v>
+        <v>245</v>
       </c>
       <c r="E11" t="s">
-        <v>221</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>5</v>
+        <v>246</v>
+      </c>
+      <c r="F11" t="s">
+        <v>14</v>
       </c>
       <c r="G11" t="s">
         <v>14</v>
       </c>
       <c r="H11" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B12" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C12" t="s">
-        <v>229</v>
+        <v>213</v>
       </c>
       <c r="D12" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
       <c r="E12" t="s">
-        <v>230</v>
-      </c>
-      <c r="F12" t="s">
-        <v>14</v>
+        <v>215</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="G12" t="s">
         <v>14</v>
       </c>
       <c r="H12" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>212</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>223</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>221</v>
       </c>
       <c r="E13" t="s">
-        <v>25</v>
+        <v>224</v>
       </c>
       <c r="F13" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="G13" t="s">
         <v>14</v>
       </c>
       <c r="H13" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -1655,13 +1674,13 @@
         <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="D14" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="E14" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="F14" t="s">
         <v>5</v>
@@ -1670,7 +1689,7 @@
         <v>14</v>
       </c>
       <c r="H14" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -1681,16 +1700,16 @@
         <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D15" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E15" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F15" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="G15" t="s">
         <v>14</v>
@@ -1707,22 +1726,22 @@
         <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="D16" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="E16" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="F16" t="s">
-        <v>55</v>
+        <v>14</v>
       </c>
       <c r="G16" t="s">
         <v>14</v>
       </c>
       <c r="H16" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -1733,22 +1752,22 @@
         <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="D17" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="E17" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="F17" t="s">
-        <v>5</v>
+        <v>54</v>
       </c>
       <c r="G17" t="s">
-        <v>14</v>
+        <v>87</v>
       </c>
       <c r="H17" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -1759,13 +1778,13 @@
         <v>23</v>
       </c>
       <c r="C18" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="D18" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E18" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="F18" t="s">
         <v>5</v>
@@ -1785,13 +1804,13 @@
         <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D19" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="E19" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="F19" t="s">
         <v>5</v>
@@ -1811,22 +1830,22 @@
         <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D20" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E20" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F20" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="G20" t="s">
-        <v>88</v>
+        <v>14</v>
       </c>
       <c r="H20" t="s">
-        <v>89</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -1837,22 +1856,22 @@
         <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D21" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="E21" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="F21" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="G21" t="s">
-        <v>14</v>
+        <v>87</v>
       </c>
       <c r="H21" t="s">
-        <v>15</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
@@ -1863,16 +1882,16 @@
         <v>23</v>
       </c>
       <c r="C22" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="D22" t="s">
-        <v>102</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>261</v>
+        <v>90</v>
+      </c>
+      <c r="E22" t="s">
+        <v>91</v>
       </c>
       <c r="F22" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="G22" t="s">
         <v>14</v>
@@ -1889,13 +1908,13 @@
         <v>23</v>
       </c>
       <c r="C23" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="D23" t="s">
-        <v>114</v>
-      </c>
-      <c r="E23" t="s">
-        <v>115</v>
+        <v>101</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>253</v>
       </c>
       <c r="F23" t="s">
         <v>14</v>
@@ -1915,13 +1934,13 @@
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D24" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="E24" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="F24" t="s">
         <v>14</v>
@@ -1941,13 +1960,13 @@
         <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D25" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E25" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F25" t="s">
         <v>14</v>
@@ -1967,13 +1986,13 @@
         <v>23</v>
       </c>
       <c r="C26" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D26" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E26" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="F26" t="s">
         <v>14</v>
@@ -1993,13 +2012,13 @@
         <v>23</v>
       </c>
       <c r="C27" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="D27" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="E27" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="F27" t="s">
         <v>14</v>
@@ -2019,13 +2038,13 @@
         <v>23</v>
       </c>
       <c r="C28" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="D28" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="E28" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="F28" t="s">
         <v>14</v>
@@ -2045,13 +2064,13 @@
         <v>23</v>
       </c>
       <c r="C29" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="D29" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E29" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="F29" t="s">
         <v>14</v>
@@ -2071,16 +2090,16 @@
         <v>23</v>
       </c>
       <c r="C30" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D30" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E30" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F30" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G30" t="s">
         <v>14</v>
@@ -2097,16 +2116,16 @@
         <v>23</v>
       </c>
       <c r="C31" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D31" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E31" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="F31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G31" t="s">
         <v>14</v>
@@ -2123,16 +2142,16 @@
         <v>23</v>
       </c>
       <c r="C32" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D32" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E32" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="F32" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G32" t="s">
         <v>14</v>
@@ -2149,13 +2168,13 @@
         <v>23</v>
       </c>
       <c r="C33" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D33" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="E33" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="F33" t="s">
         <v>13</v>
@@ -2175,16 +2194,16 @@
         <v>23</v>
       </c>
       <c r="C34" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D34" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="E34" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="F34" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G34" t="s">
         <v>14</v>
@@ -2201,13 +2220,13 @@
         <v>23</v>
       </c>
       <c r="C35" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D35" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="E35" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="F35" t="s">
         <v>14</v>
@@ -2227,13 +2246,13 @@
         <v>23</v>
       </c>
       <c r="C36" t="s">
-        <v>178</v>
+        <v>159</v>
       </c>
       <c r="D36" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
       <c r="E36" t="s">
-        <v>180</v>
+        <v>161</v>
       </c>
       <c r="F36" t="s">
         <v>14</v>
@@ -2253,13 +2272,13 @@
         <v>23</v>
       </c>
       <c r="C37" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D37" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E37" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="F37" t="s">
         <v>14</v>
@@ -2268,7 +2287,7 @@
         <v>14</v>
       </c>
       <c r="H37" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
@@ -2279,19 +2298,19 @@
         <v>23</v>
       </c>
       <c r="C38" t="s">
-        <v>186</v>
+        <v>257</v>
       </c>
       <c r="D38" t="s">
-        <v>187</v>
+        <v>258</v>
       </c>
       <c r="E38" t="s">
-        <v>188</v>
+        <v>259</v>
       </c>
       <c r="F38" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="G38" t="s">
-        <v>14</v>
+        <v>87</v>
       </c>
       <c r="H38" t="s">
         <v>22</v>
@@ -2305,19 +2324,19 @@
         <v>23</v>
       </c>
       <c r="C39" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="D39" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="E39" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="F39" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="G39" t="s">
-        <v>14</v>
+        <v>87</v>
       </c>
       <c r="H39" t="s">
         <v>22</v>
@@ -2331,13 +2350,13 @@
         <v>23</v>
       </c>
       <c r="C40" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="D40" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="E40" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="F40" t="s">
         <v>5</v>
@@ -2357,13 +2376,13 @@
         <v>23</v>
       </c>
       <c r="C41" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="D41" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="E41" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="F41" t="s">
         <v>5</v>
@@ -2383,13 +2402,13 @@
         <v>23</v>
       </c>
       <c r="C42" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
       <c r="D42" t="s">
-        <v>213</v>
+        <v>195</v>
       </c>
       <c r="E42" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
       <c r="F42" t="s">
         <v>5</v>
@@ -2398,7 +2417,7 @@
         <v>14</v>
       </c>
       <c r="H42" t="s">
-        <v>89</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
@@ -2406,25 +2425,25 @@
         <v>8</v>
       </c>
       <c r="B43" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="C43" t="s">
-        <v>10</v>
+        <v>206</v>
       </c>
       <c r="D43" t="s">
-        <v>11</v>
+        <v>207</v>
       </c>
       <c r="E43" t="s">
-        <v>12</v>
+        <v>208</v>
       </c>
       <c r="F43" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="G43" t="s">
-        <v>14</v>
+        <v>87</v>
       </c>
       <c r="H43" t="s">
-        <v>15</v>
+        <v>88</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
@@ -2435,16 +2454,16 @@
         <v>9</v>
       </c>
       <c r="C44" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D44" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E44" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F44" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="G44" t="s">
         <v>14</v>
@@ -2461,22 +2480,22 @@
         <v>9</v>
       </c>
       <c r="C45" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D45" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E45" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F45" t="s">
         <v>5</v>
       </c>
       <c r="G45" t="s">
-        <v>14</v>
+        <v>263</v>
       </c>
       <c r="H45" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
@@ -2487,22 +2506,22 @@
         <v>9</v>
       </c>
       <c r="C46" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D46" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="E46" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="F46" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="G46" t="s">
         <v>14</v>
       </c>
       <c r="H46" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
@@ -2513,13 +2532,13 @@
         <v>9</v>
       </c>
       <c r="C47" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D47" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E47" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F47" t="s">
         <v>5</v>
@@ -2528,7 +2547,7 @@
         <v>14</v>
       </c>
       <c r="H47" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
@@ -2539,22 +2558,22 @@
         <v>9</v>
       </c>
       <c r="C48" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D48" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E48" t="s">
-        <v>34</v>
+        <v>264</v>
       </c>
       <c r="F48" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="G48" t="s">
-        <v>14</v>
+        <v>87</v>
       </c>
       <c r="H48" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
@@ -2565,13 +2584,13 @@
         <v>9</v>
       </c>
       <c r="C49" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="D49" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="E49" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="F49" t="s">
         <v>5</v>
@@ -2591,13 +2610,13 @@
         <v>9</v>
       </c>
       <c r="C50" t="s">
-        <v>231</v>
+        <v>48</v>
       </c>
       <c r="D50" t="s">
-        <v>232</v>
+        <v>49</v>
       </c>
       <c r="E50" t="s">
-        <v>233</v>
+        <v>50</v>
       </c>
       <c r="F50" t="s">
         <v>5</v>
@@ -2617,13 +2636,13 @@
         <v>9</v>
       </c>
       <c r="C51" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="D51" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="E51" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="F51" t="s">
         <v>5</v>
@@ -2643,13 +2662,13 @@
         <v>9</v>
       </c>
       <c r="C52" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="D52" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="E52" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="F52" t="s">
         <v>5</v>
@@ -2668,14 +2687,14 @@
       <c r="B53" t="s">
         <v>9</v>
       </c>
-      <c r="C53" t="s">
-        <v>56</v>
-      </c>
-      <c r="D53" t="s">
-        <v>57</v>
+      <c r="C53" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>231</v>
       </c>
       <c r="E53" t="s">
-        <v>58</v>
+        <v>230</v>
       </c>
       <c r="F53" t="s">
         <v>5</v>
@@ -2695,13 +2714,13 @@
         <v>9</v>
       </c>
       <c r="C54" t="s">
-        <v>240</v>
+        <v>55</v>
       </c>
       <c r="D54" t="s">
-        <v>241</v>
+        <v>56</v>
       </c>
       <c r="E54" t="s">
-        <v>242</v>
+        <v>57</v>
       </c>
       <c r="F54" t="s">
         <v>5</v>
@@ -2710,7 +2729,7 @@
         <v>14</v>
       </c>
       <c r="H54" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
@@ -2721,13 +2740,13 @@
         <v>9</v>
       </c>
       <c r="C55" t="s">
-        <v>65</v>
+        <v>232</v>
       </c>
       <c r="D55" t="s">
-        <v>66</v>
+        <v>233</v>
       </c>
       <c r="E55" t="s">
-        <v>67</v>
+        <v>234</v>
       </c>
       <c r="F55" t="s">
         <v>5</v>
@@ -2736,7 +2755,7 @@
         <v>14</v>
       </c>
       <c r="H55" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
@@ -2747,13 +2766,13 @@
         <v>9</v>
       </c>
       <c r="C56" t="s">
-        <v>243</v>
+        <v>64</v>
       </c>
       <c r="D56" t="s">
-        <v>244</v>
+        <v>65</v>
       </c>
       <c r="E56" t="s">
-        <v>245</v>
+        <v>66</v>
       </c>
       <c r="F56" t="s">
         <v>5</v>
@@ -2773,13 +2792,13 @@
         <v>9</v>
       </c>
       <c r="C57" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="D57" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="E57" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="F57" t="s">
         <v>5</v>
@@ -2799,16 +2818,16 @@
         <v>9</v>
       </c>
       <c r="C58" t="s">
-        <v>68</v>
+        <v>238</v>
       </c>
       <c r="D58" t="s">
-        <v>69</v>
+        <v>239</v>
       </c>
       <c r="E58" t="s">
-        <v>70</v>
+        <v>240</v>
       </c>
       <c r="F58" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="G58" t="s">
         <v>14</v>
@@ -2825,13 +2844,13 @@
         <v>9</v>
       </c>
       <c r="C59" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D59" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E59" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F59" t="s">
         <v>5</v>
@@ -2851,13 +2870,13 @@
         <v>9</v>
       </c>
       <c r="C60" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D60" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E60" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F60" t="s">
         <v>5</v>
@@ -2866,7 +2885,7 @@
         <v>14</v>
       </c>
       <c r="H60" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
@@ -2877,22 +2896,22 @@
         <v>9</v>
       </c>
       <c r="C61" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D61" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E61" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F61" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="G61" t="s">
         <v>14</v>
       </c>
       <c r="H61" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
@@ -2903,16 +2922,16 @@
         <v>9</v>
       </c>
       <c r="C62" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D62" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="E62" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="F62" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="G62" t="s">
         <v>14</v>
@@ -2929,16 +2948,16 @@
         <v>9</v>
       </c>
       <c r="C63" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D63" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="E63" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F63" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="G63" t="s">
         <v>14</v>
@@ -2955,13 +2974,13 @@
         <v>9</v>
       </c>
       <c r="C64" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D64" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E64" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F64" t="s">
         <v>14</v>
@@ -2981,13 +3000,13 @@
         <v>9</v>
       </c>
       <c r="C65" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D65" t="s">
-        <v>102</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>260</v>
+        <v>98</v>
+      </c>
+      <c r="E65" t="s">
+        <v>99</v>
       </c>
       <c r="F65" t="s">
         <v>14</v>
@@ -3007,13 +3026,13 @@
         <v>9</v>
       </c>
       <c r="C66" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D66" t="s">
-        <v>105</v>
-      </c>
-      <c r="E66" t="s">
-        <v>106</v>
+        <v>101</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>252</v>
       </c>
       <c r="F66" t="s">
         <v>14</v>
@@ -3033,13 +3052,13 @@
         <v>9</v>
       </c>
       <c r="C67" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D67" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E67" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F67" t="s">
         <v>14</v>
@@ -3059,16 +3078,16 @@
         <v>9</v>
       </c>
       <c r="C68" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D68" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E68" t="s">
-        <v>112</v>
-      </c>
-      <c r="F68" t="s">
-        <v>14</v>
+        <v>108</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="G68" t="s">
         <v>14</v>
@@ -3085,16 +3104,16 @@
         <v>9</v>
       </c>
       <c r="C69" t="s">
-        <v>249</v>
+        <v>109</v>
       </c>
       <c r="D69" t="s">
-        <v>250</v>
+        <v>110</v>
       </c>
       <c r="E69" t="s">
-        <v>251</v>
-      </c>
-      <c r="F69" t="s">
-        <v>14</v>
+        <v>111</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="G69" t="s">
         <v>14</v>
@@ -3111,13 +3130,13 @@
         <v>9</v>
       </c>
       <c r="C70" t="s">
-        <v>116</v>
+        <v>241</v>
       </c>
       <c r="D70" t="s">
-        <v>114</v>
+        <v>242</v>
       </c>
       <c r="E70" t="s">
-        <v>117</v>
+        <v>243</v>
       </c>
       <c r="F70" t="s">
         <v>14</v>
@@ -3137,13 +3156,13 @@
         <v>9</v>
       </c>
       <c r="C71" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="D71" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="E71" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="F71" t="s">
         <v>14</v>
@@ -3163,13 +3182,13 @@
         <v>9</v>
       </c>
       <c r="C72" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D72" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="E72" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="F72" t="s">
         <v>14</v>
@@ -3189,13 +3208,13 @@
         <v>9</v>
       </c>
       <c r="C73" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="D73" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E73" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="F73" t="s">
         <v>14</v>
@@ -3215,13 +3234,13 @@
         <v>9</v>
       </c>
       <c r="C74" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="D74" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="E74" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="F74" t="s">
         <v>14</v>
@@ -3241,16 +3260,16 @@
         <v>9</v>
       </c>
       <c r="C75" t="s">
-        <v>163</v>
+        <v>139</v>
       </c>
       <c r="D75" t="s">
-        <v>164</v>
+        <v>137</v>
       </c>
       <c r="E75" t="s">
-        <v>165</v>
-      </c>
-      <c r="F75" t="s">
-        <v>14</v>
+        <v>140</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="G75" t="s">
         <v>14</v>
@@ -3267,16 +3286,16 @@
         <v>9</v>
       </c>
       <c r="C76" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D76" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E76" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="F76" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G76" t="s">
         <v>14</v>
@@ -3293,13 +3312,13 @@
         <v>9</v>
       </c>
       <c r="C77" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D77" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E77" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="F77" t="s">
         <v>13</v>
@@ -3319,16 +3338,16 @@
         <v>9</v>
       </c>
       <c r="C78" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D78" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E78" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="F78" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G78" t="s">
         <v>14</v>
@@ -3345,16 +3364,16 @@
         <v>9</v>
       </c>
       <c r="C79" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D79" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E79" t="s">
-        <v>177</v>
-      </c>
-      <c r="F79" t="s">
-        <v>13</v>
+        <v>173</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="G79" t="s">
         <v>14</v>
@@ -3371,22 +3390,22 @@
         <v>9</v>
       </c>
       <c r="C80" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="D80" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="E80" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="F80" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="G80" t="s">
         <v>14</v>
       </c>
       <c r="H80" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.3">
@@ -3397,16 +3416,16 @@
         <v>9</v>
       </c>
       <c r="C81" t="s">
-        <v>189</v>
+        <v>260</v>
       </c>
       <c r="D81" t="s">
-        <v>187</v>
+        <v>261</v>
       </c>
       <c r="E81" t="s">
-        <v>190</v>
+        <v>262</v>
       </c>
       <c r="F81" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="G81" t="s">
         <v>14</v>
@@ -3423,16 +3442,16 @@
         <v>9</v>
       </c>
       <c r="C82" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="D82" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="E82" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="F82" t="s">
-        <v>55</v>
+        <v>5</v>
       </c>
       <c r="G82" t="s">
         <v>14</v>
@@ -3449,19 +3468,19 @@
         <v>9</v>
       </c>
       <c r="C83" t="s">
-        <v>203</v>
+        <v>185</v>
       </c>
       <c r="D83" t="s">
-        <v>204</v>
+        <v>186</v>
       </c>
       <c r="E83" t="s">
-        <v>205</v>
+        <v>187</v>
       </c>
       <c r="F83" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
       <c r="G83" t="s">
-        <v>14</v>
+        <v>87</v>
       </c>
       <c r="H83" t="s">
         <v>22</v>
@@ -3475,13 +3494,13 @@
         <v>9</v>
       </c>
       <c r="C84" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="D84" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="E84" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="F84" t="s">
         <v>5</v>
@@ -3501,21 +3520,47 @@
         <v>9</v>
       </c>
       <c r="C85" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="D85" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="E85" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="F85" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="G85" t="s">
         <v>14</v>
       </c>
       <c r="H85" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>8</v>
+      </c>
+      <c r="B86" t="s">
+        <v>9</v>
+      </c>
+      <c r="C86" t="s">
+        <v>203</v>
+      </c>
+      <c r="D86" t="s">
+        <v>204</v>
+      </c>
+      <c r="E86" t="s">
+        <v>205</v>
+      </c>
+      <c r="F86" t="s">
+        <v>14</v>
+      </c>
+      <c r="G86" t="s">
+        <v>14</v>
+      </c>
+      <c r="H86" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Have made it through re-running 4.1.R up to creating subplot2 with the changes from manual Excel edits
</commit_message>
<xml_diff>
--- a/Sonoran-data/data-wrangling-intermediate/01b_edited7_location-dependent-manual-fix.xlsx
+++ b/Sonoran-data/data-wrangling-intermediate/01b_edited7_location-dependent-manual-fix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eltnmsu-my.sharepoint.com/personal/lossanna_nmsu_edu/Documents/Documents/02_RestoreNet/RestoreNet/Sonoran-data/data-wrangling-intermediate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="92" documentId="8_{C3EF6CDF-594F-4BE4-9EF4-7E0609E88FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1DF47B9E-8CD2-4653-8FF1-C07A2D38710F}"/>
+  <xr:revisionPtr revIDLastSave="119" documentId="8_{C3EF6CDF-594F-4BE4-9EF4-7E0609E88FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E9BE22A-AD26-4484-A1E3-EF4AE9D3D69D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{A09795D3-E60D-44CB-9C72-087875526995}"/>
   </bookViews>
@@ -872,10 +872,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1316,7 +1315,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L23" sqref="L23"/>
+      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1325,7 +1324,7 @@
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="66.44140625" customWidth="1"/>
+    <col min="5" max="5" width="81.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -1448,8 +1447,8 @@
       <c r="E5" t="s">
         <v>211</v>
       </c>
-      <c r="F5" t="s">
-        <v>14</v>
+      <c r="F5" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="G5" t="s">
         <v>14</v>
@@ -2690,7 +2689,7 @@
       <c r="C53" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="D53" t="s">
         <v>231</v>
       </c>
       <c r="E53" t="s">

</xml_diff>